<commit_message>
ECP-1125: sets up fixtures for turnover aggregation scenario 1
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImportForAggregated.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImportForAggregated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635FA4FA-31B1-374F-A0EF-4B973B4D94FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D664A5-D010-1445-B4C7-8D6C7042E023}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="32940" windowHeight="17900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="24">
   <si>
     <t>OXF-001</t>
   </si>
@@ -96,7 +96,7 @@
     <t>Reported By</t>
   </si>
   <si>
-    <t>OXF-002</t>
+    <t>OXF-TOPM2</t>
   </si>
 </sst>
 </file>
@@ -744,7 +744,7 @@
   <dimension ref="A1:R60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49:J60"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -882,6 +882,9 @@
       <c r="J3" s="6">
         <v>562</v>
       </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
@@ -907,6 +910,9 @@
         <v>62000</v>
       </c>
       <c r="J4" s="6"/>
+      <c r="L4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
@@ -933,6 +939,9 @@
       <c r="J5" s="6">
         <v>353</v>
       </c>
+      <c r="L5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
@@ -956,6 +965,9 @@
       <c r="G6" s="6">
         <v>52115</v>
       </c>
+      <c r="L6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
@@ -979,6 +991,9 @@
       <c r="G7" s="6">
         <v>76342</v>
       </c>
+      <c r="L7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
@@ -1002,6 +1017,9 @@
       <c r="G8" s="6">
         <v>70023</v>
       </c>
+      <c r="L8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
@@ -1028,6 +1046,9 @@
       <c r="J9" s="6">
         <v>0</v>
       </c>
+      <c r="L9" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
@@ -1054,6 +1075,9 @@
       <c r="J10" s="6">
         <v>442</v>
       </c>
+      <c r="L10" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
@@ -1080,6 +1104,9 @@
       <c r="J11" s="6">
         <v>688</v>
       </c>
+      <c r="L11" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -1106,6 +1133,9 @@
       <c r="J12" s="6">
         <v>970</v>
       </c>
+      <c r="L12" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
@@ -1132,6 +1162,9 @@
       <c r="J13" s="6">
         <v>744</v>
       </c>
+      <c r="L13" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
@@ -1158,6 +1191,9 @@
       <c r="J14" s="6">
         <v>746</v>
       </c>
+      <c r="L14" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
@@ -1184,6 +1220,9 @@
       <c r="J15" s="6">
         <v>614</v>
       </c>
+      <c r="L15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
@@ -1210,8 +1249,11 @@
       <c r="J16" s="6">
         <v>579</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1236,8 +1278,11 @@
       <c r="J17" s="6">
         <v>431</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1262,8 +1307,11 @@
       <c r="J18" s="6">
         <v>763</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1288,8 +1336,11 @@
       <c r="J19" s="6">
         <v>804</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1314,8 +1365,11 @@
       <c r="J20" s="6">
         <v>682</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1340,8 +1394,11 @@
       <c r="J21" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1366,8 +1423,11 @@
       <c r="J22" s="6">
         <v>532</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -1392,8 +1452,11 @@
       <c r="J23" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1418,8 +1481,11 @@
       <c r="J24" s="6">
         <v>1013</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -1444,8 +1510,11 @@
       <c r="J25" s="6">
         <v>685</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1470,8 +1539,11 @@
       <c r="J26" s="6">
         <v>688</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1496,8 +1568,11 @@
       <c r="J27" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -1522,8 +1597,11 @@
       <c r="J28" s="6">
         <v>642</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1548,8 +1626,11 @@
       <c r="J29" s="6">
         <v>526</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -1574,8 +1655,11 @@
       <c r="J30" s="6">
         <v>768</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1600,8 +1684,11 @@
       <c r="J31" s="6">
         <v>885</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1626,8 +1713,11 @@
       <c r="J32" s="6">
         <v>599</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -1652,8 +1742,11 @@
       <c r="J33" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -1678,8 +1771,11 @@
       <c r="J34" s="6">
         <v>665</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -1704,8 +1800,11 @@
       <c r="J35" s="6">
         <v>618</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -1730,8 +1829,11 @@
       <c r="J36" s="6">
         <v>894</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -1756,8 +1858,11 @@
       <c r="J37" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -1782,8 +1887,11 @@
       <c r="J38" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -1808,8 +1916,11 @@
       <c r="J39" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -1834,8 +1945,11 @@
       <c r="J40" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -1860,8 +1974,11 @@
       <c r="J41" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -1886,8 +2003,11 @@
       <c r="J42" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -1912,8 +2032,11 @@
       <c r="J43" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -1938,8 +2061,11 @@
       <c r="J44" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -1964,8 +2090,11 @@
       <c r="J45" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -1990,8 +2119,11 @@
       <c r="J46" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L46" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -2016,8 +2148,11 @@
       <c r="J47" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -2042,8 +2177,11 @@
       <c r="J48" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -2068,8 +2206,11 @@
       <c r="J49" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L49" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -2094,8 +2235,11 @@
       <c r="J50" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L50" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -2120,8 +2264,11 @@
       <c r="J51" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -2146,8 +2293,11 @@
       <c r="J52" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -2172,8 +2322,11 @@
       <c r="J53" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -2198,8 +2351,11 @@
       <c r="J54" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -2224,8 +2380,11 @@
       <c r="J55" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L55" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -2250,8 +2409,11 @@
       <c r="J56" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L56" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -2276,8 +2438,11 @@
       <c r="J57" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -2302,8 +2467,11 @@
       <c r="J58" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L58" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -2328,8 +2496,11 @@
       <c r="J59" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -2353,6 +2524,9 @@
       </c>
       <c r="J60" s="6">
         <v>0</v>
+      </c>
+      <c r="L60" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ECP-1125: sets up parallel unit with turnovers as well
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImportForAggregated.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImportForAggregated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D664A5-D010-1445-B4C7-8D6C7042E023}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4425F22-514D-A74B-9D4E-77EC2ED6D0D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="32940" windowHeight="17900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="25">
   <si>
     <t>OXF-001</t>
   </si>
@@ -96,7 +96,10 @@
     <t>Reported By</t>
   </si>
   <si>
-    <t>OXF-TOPM2</t>
+    <t>OXF-001A</t>
+  </si>
+  <si>
+    <t>OXF-001A-PAR</t>
   </si>
 </sst>
 </file>
@@ -741,16 +744,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R60"/>
+  <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -825,12 +826,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1">
         <v>42842</v>
@@ -845,23 +846,28 @@
         <v>4</v>
       </c>
       <c r="G2" s="6">
-        <v>65264</v>
+        <v>12345</v>
       </c>
       <c r="H2" s="2"/>
       <c r="J2" s="6">
-        <v>490</v>
+        <v>123</v>
       </c>
       <c r="L2" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+    </row>
+    <row r="3" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1">
         <v>42842</v>
@@ -876,23 +882,28 @@
         <v>4</v>
       </c>
       <c r="G3" s="6">
-        <v>76229</v>
+        <v>12346</v>
       </c>
       <c r="H3" s="2"/>
       <c r="J3" s="6">
-        <v>562</v>
+        <v>124</v>
       </c>
       <c r="L3" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1">
         <v>42842</v>
@@ -907,19 +918,27 @@
         <v>4</v>
       </c>
       <c r="G4" s="6">
-        <v>62000</v>
-      </c>
-      <c r="J4" s="6"/>
+        <v>12347</v>
+      </c>
+      <c r="J4" s="6">
+        <v>125</v>
+      </c>
       <c r="L4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1">
         <v>42842</v>
@@ -934,21 +953,27 @@
         <v>4</v>
       </c>
       <c r="G5" s="6">
-        <v>37473</v>
+        <v>12348</v>
       </c>
       <c r="J5" s="6">
-        <v>353</v>
+        <v>126</v>
       </c>
       <c r="L5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1">
         <v>42842</v>
@@ -963,18 +988,27 @@
         <v>4</v>
       </c>
       <c r="G6" s="6">
-        <v>52115</v>
+        <v>12349</v>
+      </c>
+      <c r="J6">
+        <v>127</v>
       </c>
       <c r="L6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1">
         <v>42842</v>
@@ -989,18 +1023,27 @@
         <v>4</v>
       </c>
       <c r="G7" s="6">
-        <v>76342</v>
+        <v>12340</v>
+      </c>
+      <c r="J7">
+        <v>128</v>
       </c>
       <c r="L7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1">
         <v>42842</v>
@@ -1015,21 +1058,30 @@
         <v>4</v>
       </c>
       <c r="G8" s="6">
-        <v>70023</v>
+        <v>12341</v>
+      </c>
+      <c r="J8">
+        <v>129</v>
       </c>
       <c r="L8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>0</v>
+      <c r="B9" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="C9" s="1">
-        <v>40374</v>
+        <v>42842</v>
       </c>
       <c r="D9" s="5">
         <v>43556</v>
@@ -1041,27 +1093,33 @@
         <v>4</v>
       </c>
       <c r="G9" s="6">
-        <v>52775</v>
+        <v>12342</v>
       </c>
       <c r="J9" s="6">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="L9" t="s">
         <v>3</v>
       </c>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
-        <v>0</v>
+      <c r="B10" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C10" s="1">
-        <v>40374</v>
+        <v>42842</v>
       </c>
       <c r="D10" s="5">
-        <v>43525</v>
+        <v>43770</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
@@ -1070,27 +1128,29 @@
         <v>4</v>
       </c>
       <c r="G10" s="6">
-        <v>58196</v>
-      </c>
+        <v>65264</v>
+      </c>
+      <c r="H10" s="2"/>
       <c r="J10" s="6">
-        <v>442</v>
+        <v>490</v>
       </c>
       <c r="L10" t="s">
         <v>3</v>
       </c>
+      <c r="N10" s="3"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
-        <v>0</v>
+      <c r="B11" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C11" s="1">
-        <v>40374</v>
+        <v>42842</v>
       </c>
       <c r="D11" s="5">
-        <v>43497</v>
+        <v>43739</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
@@ -1099,27 +1159,29 @@
         <v>4</v>
       </c>
       <c r="G11" s="6">
-        <v>66964</v>
-      </c>
+        <v>76229</v>
+      </c>
+      <c r="H11" s="2"/>
       <c r="J11" s="6">
-        <v>688</v>
+        <v>562</v>
       </c>
       <c r="L11" t="s">
         <v>3</v>
       </c>
+      <c r="N11" s="3"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
-        <v>0</v>
+      <c r="B12" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C12" s="1">
-        <v>40374</v>
+        <v>42842</v>
       </c>
       <c r="D12" s="5">
-        <v>43466</v>
+        <v>43709</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
@@ -1128,11 +1190,9 @@
         <v>4</v>
       </c>
       <c r="G12" s="6">
-        <v>93836</v>
-      </c>
-      <c r="J12" s="6">
-        <v>970</v>
-      </c>
+        <v>62000</v>
+      </c>
+      <c r="J12" s="6"/>
       <c r="L12" t="s">
         <v>3</v>
       </c>
@@ -1141,14 +1201,14 @@
       <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="B13" t="s">
-        <v>0</v>
+      <c r="B13" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C13" s="1">
-        <v>40374</v>
+        <v>42842</v>
       </c>
       <c r="D13" s="5">
-        <v>43435</v>
+        <v>43678</v>
       </c>
       <c r="E13" t="s">
         <v>1</v>
@@ -1157,10 +1217,10 @@
         <v>4</v>
       </c>
       <c r="G13" s="6">
-        <v>82688</v>
+        <v>37473</v>
       </c>
       <c r="J13" s="6">
-        <v>744</v>
+        <v>353</v>
       </c>
       <c r="L13" t="s">
         <v>3</v>
@@ -1170,14 +1230,14 @@
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" t="s">
-        <v>0</v>
+      <c r="B14" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C14" s="1">
-        <v>40374</v>
+        <v>42842</v>
       </c>
       <c r="D14" s="5">
-        <v>43405</v>
+        <v>43647</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
@@ -1186,10 +1246,7 @@
         <v>4</v>
       </c>
       <c r="G14" s="6">
-        <v>100042</v>
-      </c>
-      <c r="J14" s="6">
-        <v>746</v>
+        <v>52115</v>
       </c>
       <c r="L14" t="s">
         <v>3</v>
@@ -1199,14 +1256,14 @@
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" t="s">
-        <v>0</v>
+      <c r="B15" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C15" s="1">
-        <v>40374</v>
+        <v>42842</v>
       </c>
       <c r="D15" s="5">
-        <v>43374</v>
+        <v>43617</v>
       </c>
       <c r="E15" t="s">
         <v>1</v>
@@ -1215,10 +1272,7 @@
         <v>4</v>
       </c>
       <c r="G15" s="6">
-        <v>78646</v>
-      </c>
-      <c r="J15" s="6">
-        <v>614</v>
+        <v>76342</v>
       </c>
       <c r="L15" t="s">
         <v>3</v>
@@ -1228,14 +1282,14 @@
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" t="s">
-        <v>0</v>
+      <c r="B16" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C16" s="1">
-        <v>40374</v>
+        <v>42842</v>
       </c>
       <c r="D16" s="5">
-        <v>43344</v>
+        <v>43586</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
@@ -1244,10 +1298,7 @@
         <v>4</v>
       </c>
       <c r="G16" s="6">
-        <v>73385</v>
-      </c>
-      <c r="J16" s="6">
-        <v>579</v>
+        <v>70023</v>
       </c>
       <c r="L16" t="s">
         <v>3</v>
@@ -1264,7 +1315,7 @@
         <v>40374</v>
       </c>
       <c r="D17" s="5">
-        <v>43313</v>
+        <v>43556</v>
       </c>
       <c r="E17" t="s">
         <v>1</v>
@@ -1273,10 +1324,10 @@
         <v>4</v>
       </c>
       <c r="G17" s="6">
-        <v>50718</v>
+        <v>52775</v>
       </c>
       <c r="J17" s="6">
-        <v>431</v>
+        <v>0</v>
       </c>
       <c r="L17" t="s">
         <v>3</v>
@@ -1293,7 +1344,7 @@
         <v>40374</v>
       </c>
       <c r="D18" s="5">
-        <v>43282</v>
+        <v>43525</v>
       </c>
       <c r="E18" t="s">
         <v>1</v>
@@ -1302,10 +1353,10 @@
         <v>4</v>
       </c>
       <c r="G18" s="6">
-        <v>63506</v>
+        <v>58196</v>
       </c>
       <c r="J18" s="6">
-        <v>763</v>
+        <v>442</v>
       </c>
       <c r="L18" t="s">
         <v>3</v>
@@ -1322,7 +1373,7 @@
         <v>40374</v>
       </c>
       <c r="D19" s="5">
-        <v>43252</v>
+        <v>43497</v>
       </c>
       <c r="E19" t="s">
         <v>1</v>
@@ -1331,10 +1382,10 @@
         <v>4</v>
       </c>
       <c r="G19" s="6">
-        <v>79034</v>
+        <v>66964</v>
       </c>
       <c r="J19" s="6">
-        <v>804</v>
+        <v>688</v>
       </c>
       <c r="L19" t="s">
         <v>3</v>
@@ -1351,7 +1402,7 @@
         <v>40374</v>
       </c>
       <c r="D20" s="5">
-        <v>43221</v>
+        <v>43466</v>
       </c>
       <c r="E20" t="s">
         <v>1</v>
@@ -1360,10 +1411,10 @@
         <v>4</v>
       </c>
       <c r="G20" s="6">
-        <v>80934</v>
+        <v>93836</v>
       </c>
       <c r="J20" s="6">
-        <v>682</v>
+        <v>970</v>
       </c>
       <c r="L20" t="s">
         <v>3</v>
@@ -1380,7 +1431,7 @@
         <v>40374</v>
       </c>
       <c r="D21" s="5">
-        <v>43191</v>
+        <v>43435</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
@@ -1389,10 +1440,10 @@
         <v>4</v>
       </c>
       <c r="G21" s="6">
-        <v>68878</v>
+        <v>82688</v>
       </c>
       <c r="J21" s="6">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="L21" t="s">
         <v>3</v>
@@ -1409,7 +1460,7 @@
         <v>40374</v>
       </c>
       <c r="D22" s="5">
-        <v>43160</v>
+        <v>43405</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
@@ -1418,10 +1469,10 @@
         <v>4</v>
       </c>
       <c r="G22" s="6">
-        <v>67773</v>
+        <v>100042</v>
       </c>
       <c r="J22" s="6">
-        <v>532</v>
+        <v>746</v>
       </c>
       <c r="L22" t="s">
         <v>3</v>
@@ -1438,7 +1489,7 @@
         <v>40374</v>
       </c>
       <c r="D23" s="5">
-        <v>43132</v>
+        <v>43374</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
@@ -1447,10 +1498,10 @@
         <v>4</v>
       </c>
       <c r="G23" s="6">
-        <v>60700</v>
+        <v>78646</v>
       </c>
       <c r="J23" s="6">
-        <v>0</v>
+        <v>614</v>
       </c>
       <c r="L23" t="s">
         <v>3</v>
@@ -1467,7 +1518,7 @@
         <v>40374</v>
       </c>
       <c r="D24" s="5">
-        <v>43101</v>
+        <v>43344</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
@@ -1476,10 +1527,10 @@
         <v>4</v>
       </c>
       <c r="G24" s="6">
-        <v>91408</v>
+        <v>73385</v>
       </c>
       <c r="J24" s="6">
-        <v>1013</v>
+        <v>579</v>
       </c>
       <c r="L24" t="s">
         <v>3</v>
@@ -1496,7 +1547,7 @@
         <v>40374</v>
       </c>
       <c r="D25" s="5">
-        <v>43070</v>
+        <v>43313</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
@@ -1505,10 +1556,10 @@
         <v>4</v>
       </c>
       <c r="G25" s="6">
-        <v>85446</v>
+        <v>50718</v>
       </c>
       <c r="J25" s="6">
-        <v>685</v>
+        <v>431</v>
       </c>
       <c r="L25" t="s">
         <v>3</v>
@@ -1525,7 +1576,7 @@
         <v>40374</v>
       </c>
       <c r="D26" s="5">
-        <v>43040</v>
+        <v>43282</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
@@ -1534,10 +1585,10 @@
         <v>4</v>
       </c>
       <c r="G26" s="6">
-        <v>94846</v>
+        <v>63506</v>
       </c>
       <c r="J26" s="6">
-        <v>688</v>
+        <v>763</v>
       </c>
       <c r="L26" t="s">
         <v>3</v>
@@ -1554,7 +1605,7 @@
         <v>40374</v>
       </c>
       <c r="D27" s="5">
-        <v>43009</v>
+        <v>43252</v>
       </c>
       <c r="E27" t="s">
         <v>1</v>
@@ -1563,10 +1614,10 @@
         <v>4</v>
       </c>
       <c r="G27" s="6">
-        <v>77191</v>
+        <v>79034</v>
       </c>
       <c r="J27" s="6">
-        <v>0</v>
+        <v>804</v>
       </c>
       <c r="L27" t="s">
         <v>3</v>
@@ -1583,7 +1634,7 @@
         <v>40374</v>
       </c>
       <c r="D28" s="5">
-        <v>42979</v>
+        <v>43221</v>
       </c>
       <c r="E28" t="s">
         <v>1</v>
@@ -1592,10 +1643,10 @@
         <v>4</v>
       </c>
       <c r="G28" s="6">
-        <v>84610</v>
+        <v>80934</v>
       </c>
       <c r="J28" s="6">
-        <v>642</v>
+        <v>682</v>
       </c>
       <c r="L28" t="s">
         <v>3</v>
@@ -1612,7 +1663,7 @@
         <v>40374</v>
       </c>
       <c r="D29" s="5">
-        <v>42948</v>
+        <v>43191</v>
       </c>
       <c r="E29" t="s">
         <v>1</v>
@@ -1621,10 +1672,10 @@
         <v>4</v>
       </c>
       <c r="G29" s="6">
-        <v>58912</v>
+        <v>68878</v>
       </c>
       <c r="J29" s="6">
-        <v>526</v>
+        <v>0</v>
       </c>
       <c r="L29" t="s">
         <v>3</v>
@@ -1641,7 +1692,7 @@
         <v>40374</v>
       </c>
       <c r="D30" s="5">
-        <v>42917</v>
+        <v>43160</v>
       </c>
       <c r="E30" t="s">
         <v>1</v>
@@ -1650,10 +1701,10 @@
         <v>4</v>
       </c>
       <c r="G30" s="6">
-        <v>62095</v>
+        <v>67773</v>
       </c>
       <c r="J30" s="6">
-        <v>768</v>
+        <v>532</v>
       </c>
       <c r="L30" t="s">
         <v>3</v>
@@ -1670,7 +1721,7 @@
         <v>40374</v>
       </c>
       <c r="D31" s="5">
-        <v>42887</v>
+        <v>43132</v>
       </c>
       <c r="E31" t="s">
         <v>1</v>
@@ -1679,10 +1730,10 @@
         <v>4</v>
       </c>
       <c r="G31" s="6">
-        <v>80358</v>
+        <v>60700</v>
       </c>
       <c r="J31" s="6">
-        <v>885</v>
+        <v>0</v>
       </c>
       <c r="L31" t="s">
         <v>3</v>
@@ -1699,7 +1750,7 @@
         <v>40374</v>
       </c>
       <c r="D32" s="5">
-        <v>42856</v>
+        <v>43101</v>
       </c>
       <c r="E32" t="s">
         <v>1</v>
@@ -1708,10 +1759,10 @@
         <v>4</v>
       </c>
       <c r="G32" s="6">
-        <v>71045</v>
+        <v>91408</v>
       </c>
       <c r="J32" s="6">
-        <v>599</v>
+        <v>1013</v>
       </c>
       <c r="L32" t="s">
         <v>3</v>
@@ -1728,7 +1779,7 @@
         <v>40374</v>
       </c>
       <c r="D33" s="5">
-        <v>42826</v>
+        <v>43070</v>
       </c>
       <c r="E33" t="s">
         <v>1</v>
@@ -1737,10 +1788,10 @@
         <v>4</v>
       </c>
       <c r="G33" s="6">
-        <v>27615</v>
+        <v>85446</v>
       </c>
       <c r="J33" s="6">
-        <v>0</v>
+        <v>685</v>
       </c>
       <c r="L33" t="s">
         <v>3</v>
@@ -1757,7 +1808,7 @@
         <v>40374</v>
       </c>
       <c r="D34" s="5">
-        <v>42795</v>
+        <v>43040</v>
       </c>
       <c r="E34" t="s">
         <v>1</v>
@@ -1766,10 +1817,10 @@
         <v>4</v>
       </c>
       <c r="G34" s="6">
-        <v>61362</v>
+        <v>94846</v>
       </c>
       <c r="J34" s="6">
-        <v>665</v>
+        <v>688</v>
       </c>
       <c r="L34" t="s">
         <v>3</v>
@@ -1786,7 +1837,7 @@
         <v>40374</v>
       </c>
       <c r="D35" s="5">
-        <v>42767</v>
+        <v>43009</v>
       </c>
       <c r="E35" t="s">
         <v>1</v>
@@ -1795,10 +1846,10 @@
         <v>4</v>
       </c>
       <c r="G35" s="6">
-        <v>66143</v>
+        <v>77191</v>
       </c>
       <c r="J35" s="6">
-        <v>618</v>
+        <v>0</v>
       </c>
       <c r="L35" t="s">
         <v>3</v>
@@ -1815,7 +1866,7 @@
         <v>40374</v>
       </c>
       <c r="D36" s="5">
-        <v>42736</v>
+        <v>42979</v>
       </c>
       <c r="E36" t="s">
         <v>1</v>
@@ -1824,10 +1875,10 @@
         <v>4</v>
       </c>
       <c r="G36" s="6">
-        <v>84931</v>
+        <v>84610</v>
       </c>
       <c r="J36" s="6">
-        <v>894</v>
+        <v>642</v>
       </c>
       <c r="L36" t="s">
         <v>3</v>
@@ -1844,7 +1895,7 @@
         <v>40374</v>
       </c>
       <c r="D37" s="5">
-        <v>42705</v>
+        <v>42948</v>
       </c>
       <c r="E37" t="s">
         <v>1</v>
@@ -1853,10 +1904,10 @@
         <v>4</v>
       </c>
       <c r="G37" s="6">
-        <v>82310</v>
+        <v>58912</v>
       </c>
       <c r="J37" s="6">
-        <v>0</v>
+        <v>526</v>
       </c>
       <c r="L37" t="s">
         <v>3</v>
@@ -1873,7 +1924,7 @@
         <v>40374</v>
       </c>
       <c r="D38" s="5">
-        <v>42675</v>
+        <v>42917</v>
       </c>
       <c r="E38" t="s">
         <v>1</v>
@@ -1882,10 +1933,10 @@
         <v>4</v>
       </c>
       <c r="G38" s="6">
-        <v>101018</v>
+        <v>62095</v>
       </c>
       <c r="J38" s="6">
-        <v>0</v>
+        <v>768</v>
       </c>
       <c r="L38" t="s">
         <v>3</v>
@@ -1902,7 +1953,7 @@
         <v>40374</v>
       </c>
       <c r="D39" s="5">
-        <v>42644</v>
+        <v>42887</v>
       </c>
       <c r="E39" t="s">
         <v>1</v>
@@ -1911,10 +1962,10 @@
         <v>4</v>
       </c>
       <c r="G39" s="6">
-        <v>96487</v>
+        <v>80358</v>
       </c>
       <c r="J39" s="6">
-        <v>0</v>
+        <v>885</v>
       </c>
       <c r="L39" t="s">
         <v>3</v>
@@ -1931,7 +1982,7 @@
         <v>40374</v>
       </c>
       <c r="D40" s="5">
-        <v>42614</v>
+        <v>42856</v>
       </c>
       <c r="E40" t="s">
         <v>1</v>
@@ -1940,10 +1991,10 @@
         <v>4</v>
       </c>
       <c r="G40" s="6">
-        <v>80744</v>
+        <v>71045</v>
       </c>
       <c r="J40" s="6">
-        <v>0</v>
+        <v>599</v>
       </c>
       <c r="L40" t="s">
         <v>3</v>
@@ -1960,7 +2011,7 @@
         <v>40374</v>
       </c>
       <c r="D41" s="5">
-        <v>42583</v>
+        <v>42826</v>
       </c>
       <c r="E41" t="s">
         <v>1</v>
@@ -1969,7 +2020,7 @@
         <v>4</v>
       </c>
       <c r="G41" s="6">
-        <v>56834</v>
+        <v>27615</v>
       </c>
       <c r="J41" s="6">
         <v>0</v>
@@ -1989,7 +2040,7 @@
         <v>40374</v>
       </c>
       <c r="D42" s="5">
-        <v>42552</v>
+        <v>42795</v>
       </c>
       <c r="E42" t="s">
         <v>1</v>
@@ -1998,10 +2049,10 @@
         <v>4</v>
       </c>
       <c r="G42" s="6">
-        <v>58658</v>
+        <v>61362</v>
       </c>
       <c r="J42" s="6">
-        <v>0</v>
+        <v>665</v>
       </c>
       <c r="L42" t="s">
         <v>3</v>
@@ -2018,7 +2069,7 @@
         <v>40374</v>
       </c>
       <c r="D43" s="5">
-        <v>42522</v>
+        <v>42767</v>
       </c>
       <c r="E43" t="s">
         <v>1</v>
@@ -2027,10 +2078,10 @@
         <v>4</v>
       </c>
       <c r="G43" s="6">
-        <v>83632</v>
+        <v>66143</v>
       </c>
       <c r="J43" s="6">
-        <v>0</v>
+        <v>618</v>
       </c>
       <c r="L43" t="s">
         <v>3</v>
@@ -2047,7 +2098,7 @@
         <v>40374</v>
       </c>
       <c r="D44" s="5">
-        <v>42491</v>
+        <v>42736</v>
       </c>
       <c r="E44" t="s">
         <v>1</v>
@@ -2056,10 +2107,10 @@
         <v>4</v>
       </c>
       <c r="G44" s="6">
-        <v>97706</v>
+        <v>84931</v>
       </c>
       <c r="J44" s="6">
-        <v>0</v>
+        <v>894</v>
       </c>
       <c r="L44" t="s">
         <v>3</v>
@@ -2076,7 +2127,7 @@
         <v>40374</v>
       </c>
       <c r="D45" s="5">
-        <v>42461</v>
+        <v>42705</v>
       </c>
       <c r="E45" t="s">
         <v>1</v>
@@ -2085,7 +2136,7 @@
         <v>4</v>
       </c>
       <c r="G45" s="6">
-        <v>65457</v>
+        <v>82310</v>
       </c>
       <c r="J45" s="6">
         <v>0</v>
@@ -2105,7 +2156,7 @@
         <v>40374</v>
       </c>
       <c r="D46" s="5">
-        <v>42430</v>
+        <v>42675</v>
       </c>
       <c r="E46" t="s">
         <v>1</v>
@@ -2114,7 +2165,7 @@
         <v>4</v>
       </c>
       <c r="G46" s="6">
-        <v>80452</v>
+        <v>101018</v>
       </c>
       <c r="J46" s="6">
         <v>0</v>
@@ -2134,7 +2185,7 @@
         <v>40374</v>
       </c>
       <c r="D47" s="5">
-        <v>42401</v>
+        <v>42644</v>
       </c>
       <c r="E47" t="s">
         <v>1</v>
@@ -2143,7 +2194,7 @@
         <v>4</v>
       </c>
       <c r="G47" s="6">
-        <v>65960</v>
+        <v>96487</v>
       </c>
       <c r="J47" s="6">
         <v>0</v>
@@ -2163,7 +2214,7 @@
         <v>40374</v>
       </c>
       <c r="D48" s="5">
-        <v>42370</v>
+        <v>42614</v>
       </c>
       <c r="E48" t="s">
         <v>1</v>
@@ -2172,7 +2223,7 @@
         <v>4</v>
       </c>
       <c r="G48" s="6">
-        <v>99011</v>
+        <v>80744</v>
       </c>
       <c r="J48" s="6">
         <v>0</v>
@@ -2192,7 +2243,7 @@
         <v>40374</v>
       </c>
       <c r="D49" s="5">
-        <v>42339</v>
+        <v>42583</v>
       </c>
       <c r="E49" t="s">
         <v>1</v>
@@ -2201,7 +2252,7 @@
         <v>4</v>
       </c>
       <c r="G49" s="6">
-        <v>82107</v>
+        <v>56834</v>
       </c>
       <c r="J49" s="6">
         <v>0</v>
@@ -2221,7 +2272,7 @@
         <v>40374</v>
       </c>
       <c r="D50" s="5">
-        <v>42309</v>
+        <v>42552</v>
       </c>
       <c r="E50" t="s">
         <v>1</v>
@@ -2230,7 +2281,7 @@
         <v>4</v>
       </c>
       <c r="G50" s="6">
-        <v>69586</v>
+        <v>58658</v>
       </c>
       <c r="J50" s="6">
         <v>0</v>
@@ -2250,7 +2301,7 @@
         <v>40374</v>
       </c>
       <c r="D51" s="5">
-        <v>42278</v>
+        <v>42522</v>
       </c>
       <c r="E51" t="s">
         <v>1</v>
@@ -2259,7 +2310,7 @@
         <v>4</v>
       </c>
       <c r="G51" s="6">
-        <v>90661</v>
+        <v>83632</v>
       </c>
       <c r="J51" s="6">
         <v>0</v>
@@ -2279,7 +2330,7 @@
         <v>40374</v>
       </c>
       <c r="D52" s="5">
-        <v>42248</v>
+        <v>42491</v>
       </c>
       <c r="E52" t="s">
         <v>1</v>
@@ -2288,7 +2339,7 @@
         <v>4</v>
       </c>
       <c r="G52" s="6">
-        <v>70062</v>
+        <v>97706</v>
       </c>
       <c r="J52" s="6">
         <v>0</v>
@@ -2308,7 +2359,7 @@
         <v>40374</v>
       </c>
       <c r="D53" s="5">
-        <v>42217</v>
+        <v>42461</v>
       </c>
       <c r="E53" t="s">
         <v>1</v>
@@ -2317,7 +2368,7 @@
         <v>4</v>
       </c>
       <c r="G53" s="6">
-        <v>50481</v>
+        <v>65457</v>
       </c>
       <c r="J53" s="6">
         <v>0</v>
@@ -2337,7 +2388,7 @@
         <v>40374</v>
       </c>
       <c r="D54" s="5">
-        <v>42186</v>
+        <v>42430</v>
       </c>
       <c r="E54" t="s">
         <v>1</v>
@@ -2346,7 +2397,7 @@
         <v>4</v>
       </c>
       <c r="G54" s="6">
-        <v>51280</v>
+        <v>80452</v>
       </c>
       <c r="J54" s="6">
         <v>0</v>
@@ -2366,7 +2417,7 @@
         <v>40374</v>
       </c>
       <c r="D55" s="5">
-        <v>42156</v>
+        <v>42401</v>
       </c>
       <c r="E55" t="s">
         <v>1</v>
@@ -2375,7 +2426,7 @@
         <v>4</v>
       </c>
       <c r="G55" s="6">
-        <v>80762</v>
+        <v>65960</v>
       </c>
       <c r="J55" s="6">
         <v>0</v>
@@ -2395,7 +2446,7 @@
         <v>40374</v>
       </c>
       <c r="D56" s="5">
-        <v>42125</v>
+        <v>42370</v>
       </c>
       <c r="E56" t="s">
         <v>1</v>
@@ -2404,7 +2455,7 @@
         <v>4</v>
       </c>
       <c r="G56" s="6">
-        <v>76743</v>
+        <v>99011</v>
       </c>
       <c r="J56" s="6">
         <v>0</v>
@@ -2424,7 +2475,7 @@
         <v>40374</v>
       </c>
       <c r="D57" s="5">
-        <v>42095</v>
+        <v>42339</v>
       </c>
       <c r="E57" t="s">
         <v>1</v>
@@ -2433,7 +2484,7 @@
         <v>4</v>
       </c>
       <c r="G57" s="6">
-        <v>58280</v>
+        <v>82107</v>
       </c>
       <c r="J57" s="6">
         <v>0</v>
@@ -2453,7 +2504,7 @@
         <v>40374</v>
       </c>
       <c r="D58" s="5">
-        <v>42064</v>
+        <v>42309</v>
       </c>
       <c r="E58" t="s">
         <v>1</v>
@@ -2462,7 +2513,7 @@
         <v>4</v>
       </c>
       <c r="G58" s="6">
-        <v>71969</v>
+        <v>69586</v>
       </c>
       <c r="J58" s="6">
         <v>0</v>
@@ -2482,7 +2533,7 @@
         <v>40374</v>
       </c>
       <c r="D59" s="5">
-        <v>42036</v>
+        <v>42278</v>
       </c>
       <c r="E59" t="s">
         <v>1</v>
@@ -2491,7 +2542,7 @@
         <v>4</v>
       </c>
       <c r="G59" s="6">
-        <v>57333</v>
+        <v>90661</v>
       </c>
       <c r="J59" s="6">
         <v>0</v>
@@ -2511,21 +2562,253 @@
         <v>40374</v>
       </c>
       <c r="D60" s="5">
+        <v>42248</v>
+      </c>
+      <c r="E60" t="s">
+        <v>1</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G60" s="6">
+        <v>70062</v>
+      </c>
+      <c r="J60" s="6">
+        <v>0</v>
+      </c>
+      <c r="L60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D61" s="5">
+        <v>42217</v>
+      </c>
+      <c r="E61" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G61" s="6">
+        <v>50481</v>
+      </c>
+      <c r="J61" s="6">
+        <v>0</v>
+      </c>
+      <c r="L61" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A62" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D62" s="5">
+        <v>42186</v>
+      </c>
+      <c r="E62" t="s">
+        <v>1</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G62" s="6">
+        <v>51280</v>
+      </c>
+      <c r="J62" s="6">
+        <v>0</v>
+      </c>
+      <c r="L62" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D63" s="5">
+        <v>42156</v>
+      </c>
+      <c r="E63" t="s">
+        <v>1</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G63" s="6">
+        <v>80762</v>
+      </c>
+      <c r="J63" s="6">
+        <v>0</v>
+      </c>
+      <c r="L63" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A64" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D64" s="5">
+        <v>42125</v>
+      </c>
+      <c r="E64" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G64" s="6">
+        <v>76743</v>
+      </c>
+      <c r="J64" s="6">
+        <v>0</v>
+      </c>
+      <c r="L64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D65" s="5">
+        <v>42095</v>
+      </c>
+      <c r="E65" t="s">
+        <v>1</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G65" s="6">
+        <v>58280</v>
+      </c>
+      <c r="J65" s="6">
+        <v>0</v>
+      </c>
+      <c r="L65" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D66" s="5">
+        <v>42064</v>
+      </c>
+      <c r="E66" t="s">
+        <v>1</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G66" s="6">
+        <v>71969</v>
+      </c>
+      <c r="J66" s="6">
+        <v>0</v>
+      </c>
+      <c r="L66" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D67" s="5">
+        <v>42036</v>
+      </c>
+      <c r="E67" t="s">
+        <v>1</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G67" s="6">
+        <v>57333</v>
+      </c>
+      <c r="J67" s="6">
+        <v>0</v>
+      </c>
+      <c r="L67" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D68" s="5">
         <v>42005</v>
       </c>
-      <c r="E60" t="s">
-        <v>1</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G60" s="6">
+      <c r="E68" t="s">
+        <v>1</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="6">
         <v>110615</v>
       </c>
-      <c r="J60" s="6">
-        <v>0</v>
-      </c>
-      <c r="L60" t="s">
+      <c r="J68" s="6">
+        <v>0</v>
+      </c>
+      <c r="L68" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ECP-1125: setup 2 additional parent leases
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImportForAggregated.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImportForAggregated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4425F22-514D-A74B-9D4E-77EC2ED6D0D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABFF209-12A1-714A-873D-23627FDDAE8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="32940" windowHeight="17900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="27">
   <si>
     <t>OXF-001</t>
   </si>
@@ -101,6 +101,12 @@
   <si>
     <t>OXF-001A-PAR</t>
   </si>
+  <si>
+    <t>OXF-TOPMODEL-2</t>
+  </si>
+  <si>
+    <t>OXF-TOPMODEL-3</t>
+  </si>
 </sst>
 </file>
 
@@ -283,7 +289,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
@@ -292,6 +298,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="114">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -744,9 +751,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R68"/>
+  <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -828,16 +837,16 @@
     </row>
     <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="1">
-        <v>42842</v>
+        <v>23</v>
+      </c>
+      <c r="C2" s="8">
+        <v>43971</v>
       </c>
       <c r="D2" s="5">
-        <v>43770</v>
+        <v>43983</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
@@ -845,13 +854,13 @@
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="4">
         <v>12345</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="J2" s="6">
-        <v>123</v>
-      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="L2" t="s">
         <v>3</v>
       </c>
@@ -864,16 +873,16 @@
     </row>
     <row r="3" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="1">
-        <v>42842</v>
+        <v>23</v>
+      </c>
+      <c r="C3" s="8">
+        <v>43971</v>
       </c>
       <c r="D3" s="5">
-        <v>43739</v>
+        <v>43952</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
@@ -881,13 +890,13 @@
       <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="6">
-        <v>12346</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="J3" s="6">
-        <v>124</v>
-      </c>
+      <c r="G3" s="4">
+        <v>5670</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
       <c r="L3" t="s">
         <v>3</v>
       </c>
@@ -900,16 +909,16 @@
     </row>
     <row r="4" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1">
-        <v>42842</v>
+        <v>23</v>
+      </c>
+      <c r="C4" s="8">
+        <v>43779</v>
       </c>
       <c r="D4" s="5">
-        <v>43709</v>
+        <v>43952</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -917,12 +926,13 @@
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="6">
-        <v>12347</v>
-      </c>
-      <c r="J4" s="6">
-        <v>125</v>
-      </c>
+      <c r="G4" s="4">
+        <v>7890</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
       <c r="L4" t="s">
         <v>3</v>
       </c>
@@ -935,16 +945,16 @@
     </row>
     <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="1">
-        <v>42842</v>
+        <v>23</v>
+      </c>
+      <c r="C5" s="8">
+        <v>43779</v>
       </c>
       <c r="D5" s="5">
-        <v>43678</v>
+        <v>43922</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
@@ -952,12 +962,13 @@
       <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="4">
         <v>12348</v>
       </c>
-      <c r="J5" s="6">
-        <v>126</v>
-      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
       <c r="L5" t="s">
         <v>3</v>
       </c>
@@ -970,16 +981,16 @@
     </row>
     <row r="6" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1">
-        <v>42842</v>
+        <v>23</v>
+      </c>
+      <c r="C6" s="8">
+        <v>43779</v>
       </c>
       <c r="D6" s="5">
-        <v>43647</v>
+        <v>43891</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
@@ -987,12 +998,13 @@
       <c r="F6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="6">
-        <v>12349</v>
-      </c>
-      <c r="J6">
-        <v>127</v>
-      </c>
+      <c r="G6" s="4">
+        <v>12347</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
       <c r="L6" t="s">
         <v>3</v>
       </c>
@@ -1005,16 +1017,16 @@
     </row>
     <row r="7" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1">
-        <v>42842</v>
+        <v>23</v>
+      </c>
+      <c r="C7" s="8">
+        <v>43779</v>
       </c>
       <c r="D7" s="5">
-        <v>43617</v>
+        <v>43862</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
@@ -1022,12 +1034,13 @@
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="6">
-        <v>12340</v>
-      </c>
-      <c r="J7">
-        <v>128</v>
-      </c>
+      <c r="G7" s="4">
+        <v>12346</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
       <c r="L7" t="s">
         <v>3</v>
       </c>
@@ -1040,16 +1053,16 @@
     </row>
     <row r="8" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="1">
-        <v>42842</v>
+        <v>23</v>
+      </c>
+      <c r="C8" s="8">
+        <v>43779</v>
       </c>
       <c r="D8" s="5">
-        <v>43586</v>
+        <v>43831</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
@@ -1057,12 +1070,13 @@
       <c r="F8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="6">
-        <v>12341</v>
-      </c>
-      <c r="J8">
-        <v>129</v>
-      </c>
+      <c r="G8" s="4">
+        <v>12435</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
       <c r="L8" t="s">
         <v>3</v>
       </c>
@@ -1075,16 +1089,16 @@
     </row>
     <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1">
-        <v>42842</v>
+        <v>23</v>
+      </c>
+      <c r="C9" s="8">
+        <v>43779</v>
       </c>
       <c r="D9" s="5">
-        <v>43556</v>
+        <v>43800</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
@@ -1092,12 +1106,15 @@
       <c r="F9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="6">
-        <v>12342</v>
-      </c>
-      <c r="J9" s="6">
-        <v>120</v>
-      </c>
+      <c r="G9" s="4">
+        <v>12344</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4">
+        <v>123</v>
+      </c>
+      <c r="K9" s="4"/>
       <c r="L9" t="s">
         <v>3</v>
       </c>
@@ -1108,15 +1125,15 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1">
-        <v>42842</v>
+      <c r="C10" s="8">
+        <v>43779</v>
       </c>
       <c r="D10" s="5">
         <v>43770</v>
@@ -1127,30 +1144,37 @@
       <c r="F10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="6">
-        <v>65264</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="J10" s="6">
-        <v>490</v>
-      </c>
+      <c r="G10" s="4">
+        <v>6789</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4">
+        <v>77</v>
+      </c>
+      <c r="K10" s="4"/>
       <c r="L10" t="s">
         <v>3</v>
       </c>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+    </row>
+    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1">
         <v>42842</v>
       </c>
       <c r="D11" s="5">
-        <v>43739</v>
+        <v>43770</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
@@ -1159,29 +1183,34 @@
         <v>4</v>
       </c>
       <c r="G11" s="6">
-        <v>76229</v>
+        <v>5678</v>
       </c>
       <c r="H11" s="2"/>
       <c r="J11" s="6">
-        <v>562</v>
+        <v>66</v>
       </c>
       <c r="L11" t="s">
         <v>3</v>
       </c>
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+    </row>
+    <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1">
         <v>42842</v>
       </c>
       <c r="D12" s="5">
-        <v>43709</v>
+        <v>43739</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
@@ -1190,25 +1219,34 @@
         <v>4</v>
       </c>
       <c r="G12" s="6">
-        <v>62000</v>
-      </c>
-      <c r="J12" s="6"/>
+        <v>12346</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="J12" s="6">
+        <v>124</v>
+      </c>
       <c r="L12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+    </row>
+    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1">
         <v>42842</v>
       </c>
       <c r="D13" s="5">
-        <v>43678</v>
+        <v>43709</v>
       </c>
       <c r="E13" t="s">
         <v>1</v>
@@ -1217,27 +1255,33 @@
         <v>4</v>
       </c>
       <c r="G13" s="6">
-        <v>37473</v>
+        <v>12347</v>
       </c>
       <c r="J13" s="6">
-        <v>353</v>
+        <v>125</v>
       </c>
       <c r="L13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1">
         <v>42842</v>
       </c>
       <c r="D14" s="5">
-        <v>43647</v>
+        <v>43678</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
@@ -1246,24 +1290,33 @@
         <v>4</v>
       </c>
       <c r="G14" s="6">
-        <v>52115</v>
+        <v>12348</v>
+      </c>
+      <c r="J14" s="6">
+        <v>126</v>
       </c>
       <c r="L14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1">
         <v>42842</v>
       </c>
       <c r="D15" s="5">
-        <v>43617</v>
+        <v>43647</v>
       </c>
       <c r="E15" t="s">
         <v>1</v>
@@ -1272,497 +1325,520 @@
         <v>4</v>
       </c>
       <c r="G15" s="6">
-        <v>76342</v>
+        <v>12349</v>
+      </c>
+      <c r="J15">
+        <v>127</v>
       </c>
       <c r="L15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1">
         <v>42842</v>
       </c>
       <c r="D16" s="5">
+        <v>43617</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="6">
+        <v>12340</v>
+      </c>
+      <c r="J16">
+        <v>128</v>
+      </c>
+      <c r="L16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1">
+        <v>42842</v>
+      </c>
+      <c r="D17" s="5">
         <v>43586</v>
       </c>
-      <c r="E16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="6">
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="6">
+        <v>12341</v>
+      </c>
+      <c r="J17">
+        <v>129</v>
+      </c>
+      <c r="L17" t="s">
+        <v>3</v>
+      </c>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1">
+        <v>42842</v>
+      </c>
+      <c r="D18" s="5">
+        <v>43556</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="6">
+        <v>12342</v>
+      </c>
+      <c r="J18" s="6">
+        <v>120</v>
+      </c>
+      <c r="L18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="1">
+        <v>42842</v>
+      </c>
+      <c r="D19" s="5">
+        <v>43770</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="6">
+        <v>65264</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="J19" s="6">
+        <v>490</v>
+      </c>
+      <c r="L19" t="s">
+        <v>3</v>
+      </c>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="1">
+        <v>42842</v>
+      </c>
+      <c r="D20" s="5">
+        <v>43739</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="6">
+        <v>76229</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="J20" s="6">
+        <v>562</v>
+      </c>
+      <c r="L20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="1">
+        <v>42842</v>
+      </c>
+      <c r="D21" s="5">
+        <v>43709</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="6">
+        <v>62000</v>
+      </c>
+      <c r="J21" s="6"/>
+      <c r="L21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1">
+        <v>42842</v>
+      </c>
+      <c r="D22" s="5">
+        <v>43678</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="6">
+        <v>37473</v>
+      </c>
+      <c r="J22" s="6">
+        <v>353</v>
+      </c>
+      <c r="L22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1">
+        <v>42842</v>
+      </c>
+      <c r="D23" s="5">
+        <v>43647</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="6">
+        <v>52115</v>
+      </c>
+      <c r="L23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1">
+        <v>42842</v>
+      </c>
+      <c r="D24" s="5">
+        <v>43617</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="6">
+        <v>76342</v>
+      </c>
+      <c r="L24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1">
+        <v>42842</v>
+      </c>
+      <c r="D25" s="5">
+        <v>43586</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="6">
         <v>70023</v>
       </c>
-      <c r="L16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D17" s="5">
+      <c r="L25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D26" s="5">
         <v>43556</v>
       </c>
-      <c r="E17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" s="6">
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="6">
         <v>52775</v>
       </c>
-      <c r="J17" s="6">
-        <v>0</v>
-      </c>
-      <c r="L17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D18" s="5">
+      <c r="J26" s="6">
+        <v>0</v>
+      </c>
+      <c r="L26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D27" s="5">
         <v>43525</v>
       </c>
-      <c r="E18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="6">
+      <c r="E27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="6">
         <v>58196</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J27" s="6">
         <v>442</v>
       </c>
-      <c r="L18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D19" s="5">
+      <c r="L27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D28" s="5">
         <v>43497</v>
       </c>
-      <c r="E19" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="6">
+      <c r="E28" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="6">
         <v>66964</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J28" s="6">
         <v>688</v>
       </c>
-      <c r="L19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D20" s="5">
+      <c r="L28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D29" s="5">
         <v>43466</v>
       </c>
-      <c r="E20" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="6">
+      <c r="E29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="6">
         <v>93836</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J29" s="6">
         <v>970</v>
       </c>
-      <c r="L20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D21" s="5">
+      <c r="L29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D30" s="5">
         <v>43435</v>
       </c>
-      <c r="E21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="6">
+      <c r="E30" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="6">
         <v>82688</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J30" s="6">
         <v>744</v>
       </c>
-      <c r="L21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D22" s="5">
+      <c r="L30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D31" s="5">
         <v>43405</v>
       </c>
-      <c r="E22" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22" s="6">
+      <c r="E31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="6">
         <v>100042</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J31" s="6">
         <v>746</v>
       </c>
-      <c r="L22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D23" s="5">
+      <c r="L31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D32" s="5">
         <v>43374</v>
       </c>
-      <c r="E23" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G23" s="6">
+      <c r="E32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="6">
         <v>78646</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J32" s="6">
         <v>614</v>
-      </c>
-      <c r="L23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D24" s="5">
-        <v>43344</v>
-      </c>
-      <c r="E24" t="s">
-        <v>1</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" s="6">
-        <v>73385</v>
-      </c>
-      <c r="J24" s="6">
-        <v>579</v>
-      </c>
-      <c r="L24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D25" s="5">
-        <v>43313</v>
-      </c>
-      <c r="E25" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" s="6">
-        <v>50718</v>
-      </c>
-      <c r="J25" s="6">
-        <v>431</v>
-      </c>
-      <c r="L25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D26" s="5">
-        <v>43282</v>
-      </c>
-      <c r="E26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="6">
-        <v>63506</v>
-      </c>
-      <c r="J26" s="6">
-        <v>763</v>
-      </c>
-      <c r="L26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D27" s="5">
-        <v>43252</v>
-      </c>
-      <c r="E27" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="6">
-        <v>79034</v>
-      </c>
-      <c r="J27" s="6">
-        <v>804</v>
-      </c>
-      <c r="L27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D28" s="5">
-        <v>43221</v>
-      </c>
-      <c r="E28" t="s">
-        <v>1</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" s="6">
-        <v>80934</v>
-      </c>
-      <c r="J28" s="6">
-        <v>682</v>
-      </c>
-      <c r="L28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D29" s="5">
-        <v>43191</v>
-      </c>
-      <c r="E29" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G29" s="6">
-        <v>68878</v>
-      </c>
-      <c r="J29" s="6">
-        <v>0</v>
-      </c>
-      <c r="L29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D30" s="5">
-        <v>43160</v>
-      </c>
-      <c r="E30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G30" s="6">
-        <v>67773</v>
-      </c>
-      <c r="J30" s="6">
-        <v>532</v>
-      </c>
-      <c r="L30" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D31" s="5">
-        <v>43132</v>
-      </c>
-      <c r="E31" t="s">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G31" s="6">
-        <v>60700</v>
-      </c>
-      <c r="J31" s="6">
-        <v>0</v>
-      </c>
-      <c r="L31" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A32" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="1">
-        <v>40374</v>
-      </c>
-      <c r="D32" s="5">
-        <v>43101</v>
-      </c>
-      <c r="E32" t="s">
-        <v>1</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G32" s="6">
-        <v>91408</v>
-      </c>
-      <c r="J32" s="6">
-        <v>1013</v>
       </c>
       <c r="L32" t="s">
         <v>3</v>
@@ -1779,7 +1855,7 @@
         <v>40374</v>
       </c>
       <c r="D33" s="5">
-        <v>43070</v>
+        <v>43344</v>
       </c>
       <c r="E33" t="s">
         <v>1</v>
@@ -1788,10 +1864,10 @@
         <v>4</v>
       </c>
       <c r="G33" s="6">
-        <v>85446</v>
+        <v>73385</v>
       </c>
       <c r="J33" s="6">
-        <v>685</v>
+        <v>579</v>
       </c>
       <c r="L33" t="s">
         <v>3</v>
@@ -1808,7 +1884,7 @@
         <v>40374</v>
       </c>
       <c r="D34" s="5">
-        <v>43040</v>
+        <v>43313</v>
       </c>
       <c r="E34" t="s">
         <v>1</v>
@@ -1817,10 +1893,10 @@
         <v>4</v>
       </c>
       <c r="G34" s="6">
-        <v>94846</v>
+        <v>50718</v>
       </c>
       <c r="J34" s="6">
-        <v>688</v>
+        <v>431</v>
       </c>
       <c r="L34" t="s">
         <v>3</v>
@@ -1837,7 +1913,7 @@
         <v>40374</v>
       </c>
       <c r="D35" s="5">
-        <v>43009</v>
+        <v>43282</v>
       </c>
       <c r="E35" t="s">
         <v>1</v>
@@ -1846,10 +1922,10 @@
         <v>4</v>
       </c>
       <c r="G35" s="6">
-        <v>77191</v>
+        <v>63506</v>
       </c>
       <c r="J35" s="6">
-        <v>0</v>
+        <v>763</v>
       </c>
       <c r="L35" t="s">
         <v>3</v>
@@ -1866,7 +1942,7 @@
         <v>40374</v>
       </c>
       <c r="D36" s="5">
-        <v>42979</v>
+        <v>43252</v>
       </c>
       <c r="E36" t="s">
         <v>1</v>
@@ -1875,10 +1951,10 @@
         <v>4</v>
       </c>
       <c r="G36" s="6">
-        <v>84610</v>
+        <v>79034</v>
       </c>
       <c r="J36" s="6">
-        <v>642</v>
+        <v>804</v>
       </c>
       <c r="L36" t="s">
         <v>3</v>
@@ -1895,7 +1971,7 @@
         <v>40374</v>
       </c>
       <c r="D37" s="5">
-        <v>42948</v>
+        <v>43221</v>
       </c>
       <c r="E37" t="s">
         <v>1</v>
@@ -1904,10 +1980,10 @@
         <v>4</v>
       </c>
       <c r="G37" s="6">
-        <v>58912</v>
+        <v>80934</v>
       </c>
       <c r="J37" s="6">
-        <v>526</v>
+        <v>682</v>
       </c>
       <c r="L37" t="s">
         <v>3</v>
@@ -1924,7 +2000,7 @@
         <v>40374</v>
       </c>
       <c r="D38" s="5">
-        <v>42917</v>
+        <v>43191</v>
       </c>
       <c r="E38" t="s">
         <v>1</v>
@@ -1933,10 +2009,10 @@
         <v>4</v>
       </c>
       <c r="G38" s="6">
-        <v>62095</v>
+        <v>68878</v>
       </c>
       <c r="J38" s="6">
-        <v>768</v>
+        <v>0</v>
       </c>
       <c r="L38" t="s">
         <v>3</v>
@@ -1953,7 +2029,7 @@
         <v>40374</v>
       </c>
       <c r="D39" s="5">
-        <v>42887</v>
+        <v>43160</v>
       </c>
       <c r="E39" t="s">
         <v>1</v>
@@ -1962,10 +2038,10 @@
         <v>4</v>
       </c>
       <c r="G39" s="6">
-        <v>80358</v>
+        <v>67773</v>
       </c>
       <c r="J39" s="6">
-        <v>885</v>
+        <v>532</v>
       </c>
       <c r="L39" t="s">
         <v>3</v>
@@ -1982,7 +2058,7 @@
         <v>40374</v>
       </c>
       <c r="D40" s="5">
-        <v>42856</v>
+        <v>43132</v>
       </c>
       <c r="E40" t="s">
         <v>1</v>
@@ -1991,10 +2067,10 @@
         <v>4</v>
       </c>
       <c r="G40" s="6">
-        <v>71045</v>
+        <v>60700</v>
       </c>
       <c r="J40" s="6">
-        <v>599</v>
+        <v>0</v>
       </c>
       <c r="L40" t="s">
         <v>3</v>
@@ -2011,7 +2087,7 @@
         <v>40374</v>
       </c>
       <c r="D41" s="5">
-        <v>42826</v>
+        <v>43101</v>
       </c>
       <c r="E41" t="s">
         <v>1</v>
@@ -2020,10 +2096,10 @@
         <v>4</v>
       </c>
       <c r="G41" s="6">
-        <v>27615</v>
+        <v>91408</v>
       </c>
       <c r="J41" s="6">
-        <v>0</v>
+        <v>1013</v>
       </c>
       <c r="L41" t="s">
         <v>3</v>
@@ -2040,7 +2116,7 @@
         <v>40374</v>
       </c>
       <c r="D42" s="5">
-        <v>42795</v>
+        <v>43070</v>
       </c>
       <c r="E42" t="s">
         <v>1</v>
@@ -2049,10 +2125,10 @@
         <v>4</v>
       </c>
       <c r="G42" s="6">
-        <v>61362</v>
+        <v>85446</v>
       </c>
       <c r="J42" s="6">
-        <v>665</v>
+        <v>685</v>
       </c>
       <c r="L42" t="s">
         <v>3</v>
@@ -2069,7 +2145,7 @@
         <v>40374</v>
       </c>
       <c r="D43" s="5">
-        <v>42767</v>
+        <v>43040</v>
       </c>
       <c r="E43" t="s">
         <v>1</v>
@@ -2078,10 +2154,10 @@
         <v>4</v>
       </c>
       <c r="G43" s="6">
-        <v>66143</v>
+        <v>94846</v>
       </c>
       <c r="J43" s="6">
-        <v>618</v>
+        <v>688</v>
       </c>
       <c r="L43" t="s">
         <v>3</v>
@@ -2098,7 +2174,7 @@
         <v>40374</v>
       </c>
       <c r="D44" s="5">
-        <v>42736</v>
+        <v>43009</v>
       </c>
       <c r="E44" t="s">
         <v>1</v>
@@ -2107,10 +2183,10 @@
         <v>4</v>
       </c>
       <c r="G44" s="6">
-        <v>84931</v>
+        <v>77191</v>
       </c>
       <c r="J44" s="6">
-        <v>894</v>
+        <v>0</v>
       </c>
       <c r="L44" t="s">
         <v>3</v>
@@ -2127,7 +2203,7 @@
         <v>40374</v>
       </c>
       <c r="D45" s="5">
-        <v>42705</v>
+        <v>42979</v>
       </c>
       <c r="E45" t="s">
         <v>1</v>
@@ -2136,10 +2212,10 @@
         <v>4</v>
       </c>
       <c r="G45" s="6">
-        <v>82310</v>
+        <v>84610</v>
       </c>
       <c r="J45" s="6">
-        <v>0</v>
+        <v>642</v>
       </c>
       <c r="L45" t="s">
         <v>3</v>
@@ -2156,7 +2232,7 @@
         <v>40374</v>
       </c>
       <c r="D46" s="5">
-        <v>42675</v>
+        <v>42948</v>
       </c>
       <c r="E46" t="s">
         <v>1</v>
@@ -2165,10 +2241,10 @@
         <v>4</v>
       </c>
       <c r="G46" s="6">
-        <v>101018</v>
+        <v>58912</v>
       </c>
       <c r="J46" s="6">
-        <v>0</v>
+        <v>526</v>
       </c>
       <c r="L46" t="s">
         <v>3</v>
@@ -2185,7 +2261,7 @@
         <v>40374</v>
       </c>
       <c r="D47" s="5">
-        <v>42644</v>
+        <v>42917</v>
       </c>
       <c r="E47" t="s">
         <v>1</v>
@@ -2194,10 +2270,10 @@
         <v>4</v>
       </c>
       <c r="G47" s="6">
-        <v>96487</v>
+        <v>62095</v>
       </c>
       <c r="J47" s="6">
-        <v>0</v>
+        <v>768</v>
       </c>
       <c r="L47" t="s">
         <v>3</v>
@@ -2214,7 +2290,7 @@
         <v>40374</v>
       </c>
       <c r="D48" s="5">
-        <v>42614</v>
+        <v>42887</v>
       </c>
       <c r="E48" t="s">
         <v>1</v>
@@ -2223,10 +2299,10 @@
         <v>4</v>
       </c>
       <c r="G48" s="6">
-        <v>80744</v>
+        <v>80358</v>
       </c>
       <c r="J48" s="6">
-        <v>0</v>
+        <v>885</v>
       </c>
       <c r="L48" t="s">
         <v>3</v>
@@ -2243,7 +2319,7 @@
         <v>40374</v>
       </c>
       <c r="D49" s="5">
-        <v>42583</v>
+        <v>42856</v>
       </c>
       <c r="E49" t="s">
         <v>1</v>
@@ -2252,10 +2328,10 @@
         <v>4</v>
       </c>
       <c r="G49" s="6">
-        <v>56834</v>
+        <v>71045</v>
       </c>
       <c r="J49" s="6">
-        <v>0</v>
+        <v>599</v>
       </c>
       <c r="L49" t="s">
         <v>3</v>
@@ -2272,7 +2348,7 @@
         <v>40374</v>
       </c>
       <c r="D50" s="5">
-        <v>42552</v>
+        <v>42826</v>
       </c>
       <c r="E50" t="s">
         <v>1</v>
@@ -2281,7 +2357,7 @@
         <v>4</v>
       </c>
       <c r="G50" s="6">
-        <v>58658</v>
+        <v>27615</v>
       </c>
       <c r="J50" s="6">
         <v>0</v>
@@ -2301,7 +2377,7 @@
         <v>40374</v>
       </c>
       <c r="D51" s="5">
-        <v>42522</v>
+        <v>42795</v>
       </c>
       <c r="E51" t="s">
         <v>1</v>
@@ -2310,10 +2386,10 @@
         <v>4</v>
       </c>
       <c r="G51" s="6">
-        <v>83632</v>
+        <v>61362</v>
       </c>
       <c r="J51" s="6">
-        <v>0</v>
+        <v>665</v>
       </c>
       <c r="L51" t="s">
         <v>3</v>
@@ -2330,7 +2406,7 @@
         <v>40374</v>
       </c>
       <c r="D52" s="5">
-        <v>42491</v>
+        <v>42767</v>
       </c>
       <c r="E52" t="s">
         <v>1</v>
@@ -2339,10 +2415,10 @@
         <v>4</v>
       </c>
       <c r="G52" s="6">
-        <v>97706</v>
+        <v>66143</v>
       </c>
       <c r="J52" s="6">
-        <v>0</v>
+        <v>618</v>
       </c>
       <c r="L52" t="s">
         <v>3</v>
@@ -2359,7 +2435,7 @@
         <v>40374</v>
       </c>
       <c r="D53" s="5">
-        <v>42461</v>
+        <v>42736</v>
       </c>
       <c r="E53" t="s">
         <v>1</v>
@@ -2368,10 +2444,10 @@
         <v>4</v>
       </c>
       <c r="G53" s="6">
-        <v>65457</v>
+        <v>84931</v>
       </c>
       <c r="J53" s="6">
-        <v>0</v>
+        <v>894</v>
       </c>
       <c r="L53" t="s">
         <v>3</v>
@@ -2388,7 +2464,7 @@
         <v>40374</v>
       </c>
       <c r="D54" s="5">
-        <v>42430</v>
+        <v>42705</v>
       </c>
       <c r="E54" t="s">
         <v>1</v>
@@ -2397,7 +2473,7 @@
         <v>4</v>
       </c>
       <c r="G54" s="6">
-        <v>80452</v>
+        <v>82310</v>
       </c>
       <c r="J54" s="6">
         <v>0</v>
@@ -2417,7 +2493,7 @@
         <v>40374</v>
       </c>
       <c r="D55" s="5">
-        <v>42401</v>
+        <v>42675</v>
       </c>
       <c r="E55" t="s">
         <v>1</v>
@@ -2426,7 +2502,7 @@
         <v>4</v>
       </c>
       <c r="G55" s="6">
-        <v>65960</v>
+        <v>101018</v>
       </c>
       <c r="J55" s="6">
         <v>0</v>
@@ -2446,7 +2522,7 @@
         <v>40374</v>
       </c>
       <c r="D56" s="5">
-        <v>42370</v>
+        <v>42644</v>
       </c>
       <c r="E56" t="s">
         <v>1</v>
@@ -2455,7 +2531,7 @@
         <v>4</v>
       </c>
       <c r="G56" s="6">
-        <v>99011</v>
+        <v>96487</v>
       </c>
       <c r="J56" s="6">
         <v>0</v>
@@ -2475,7 +2551,7 @@
         <v>40374</v>
       </c>
       <c r="D57" s="5">
-        <v>42339</v>
+        <v>42614</v>
       </c>
       <c r="E57" t="s">
         <v>1</v>
@@ -2484,7 +2560,7 @@
         <v>4</v>
       </c>
       <c r="G57" s="6">
-        <v>82107</v>
+        <v>80744</v>
       </c>
       <c r="J57" s="6">
         <v>0</v>
@@ -2504,7 +2580,7 @@
         <v>40374</v>
       </c>
       <c r="D58" s="5">
-        <v>42309</v>
+        <v>42583</v>
       </c>
       <c r="E58" t="s">
         <v>1</v>
@@ -2513,7 +2589,7 @@
         <v>4</v>
       </c>
       <c r="G58" s="6">
-        <v>69586</v>
+        <v>56834</v>
       </c>
       <c r="J58" s="6">
         <v>0</v>
@@ -2533,7 +2609,7 @@
         <v>40374</v>
       </c>
       <c r="D59" s="5">
-        <v>42278</v>
+        <v>42552</v>
       </c>
       <c r="E59" t="s">
         <v>1</v>
@@ -2542,7 +2618,7 @@
         <v>4</v>
       </c>
       <c r="G59" s="6">
-        <v>90661</v>
+        <v>58658</v>
       </c>
       <c r="J59" s="6">
         <v>0</v>
@@ -2562,7 +2638,7 @@
         <v>40374</v>
       </c>
       <c r="D60" s="5">
-        <v>42248</v>
+        <v>42522</v>
       </c>
       <c r="E60" t="s">
         <v>1</v>
@@ -2571,7 +2647,7 @@
         <v>4</v>
       </c>
       <c r="G60" s="6">
-        <v>70062</v>
+        <v>83632</v>
       </c>
       <c r="J60" s="6">
         <v>0</v>
@@ -2591,7 +2667,7 @@
         <v>40374</v>
       </c>
       <c r="D61" s="5">
-        <v>42217</v>
+        <v>42491</v>
       </c>
       <c r="E61" t="s">
         <v>1</v>
@@ -2600,7 +2676,7 @@
         <v>4</v>
       </c>
       <c r="G61" s="6">
-        <v>50481</v>
+        <v>97706</v>
       </c>
       <c r="J61" s="6">
         <v>0</v>
@@ -2620,7 +2696,7 @@
         <v>40374</v>
       </c>
       <c r="D62" s="5">
-        <v>42186</v>
+        <v>42461</v>
       </c>
       <c r="E62" t="s">
         <v>1</v>
@@ -2629,7 +2705,7 @@
         <v>4</v>
       </c>
       <c r="G62" s="6">
-        <v>51280</v>
+        <v>65457</v>
       </c>
       <c r="J62" s="6">
         <v>0</v>
@@ -2649,7 +2725,7 @@
         <v>40374</v>
       </c>
       <c r="D63" s="5">
-        <v>42156</v>
+        <v>42430</v>
       </c>
       <c r="E63" t="s">
         <v>1</v>
@@ -2658,7 +2734,7 @@
         <v>4</v>
       </c>
       <c r="G63" s="6">
-        <v>80762</v>
+        <v>80452</v>
       </c>
       <c r="J63" s="6">
         <v>0</v>
@@ -2678,7 +2754,7 @@
         <v>40374</v>
       </c>
       <c r="D64" s="5">
-        <v>42125</v>
+        <v>42401</v>
       </c>
       <c r="E64" t="s">
         <v>1</v>
@@ -2687,7 +2763,7 @@
         <v>4</v>
       </c>
       <c r="G64" s="6">
-        <v>76743</v>
+        <v>65960</v>
       </c>
       <c r="J64" s="6">
         <v>0</v>
@@ -2707,7 +2783,7 @@
         <v>40374</v>
       </c>
       <c r="D65" s="5">
-        <v>42095</v>
+        <v>42370</v>
       </c>
       <c r="E65" t="s">
         <v>1</v>
@@ -2716,7 +2792,7 @@
         <v>4</v>
       </c>
       <c r="G65" s="6">
-        <v>58280</v>
+        <v>99011</v>
       </c>
       <c r="J65" s="6">
         <v>0</v>
@@ -2736,7 +2812,7 @@
         <v>40374</v>
       </c>
       <c r="D66" s="5">
-        <v>42064</v>
+        <v>42339</v>
       </c>
       <c r="E66" t="s">
         <v>1</v>
@@ -2745,7 +2821,7 @@
         <v>4</v>
       </c>
       <c r="G66" s="6">
-        <v>71969</v>
+        <v>82107</v>
       </c>
       <c r="J66" s="6">
         <v>0</v>
@@ -2765,7 +2841,7 @@
         <v>40374</v>
       </c>
       <c r="D67" s="5">
-        <v>42036</v>
+        <v>42309</v>
       </c>
       <c r="E67" t="s">
         <v>1</v>
@@ -2774,7 +2850,7 @@
         <v>4</v>
       </c>
       <c r="G67" s="6">
-        <v>57333</v>
+        <v>69586</v>
       </c>
       <c r="J67" s="6">
         <v>0</v>
@@ -2794,21 +2870,282 @@
         <v>40374</v>
       </c>
       <c r="D68" s="5">
+        <v>42278</v>
+      </c>
+      <c r="E68" t="s">
+        <v>1</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="6">
+        <v>90661</v>
+      </c>
+      <c r="J68" s="6">
+        <v>0</v>
+      </c>
+      <c r="L68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A69" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D69" s="5">
+        <v>42248</v>
+      </c>
+      <c r="E69" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G69" s="6">
+        <v>70062</v>
+      </c>
+      <c r="J69" s="6">
+        <v>0</v>
+      </c>
+      <c r="L69" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D70" s="5">
+        <v>42217</v>
+      </c>
+      <c r="E70" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G70" s="6">
+        <v>50481</v>
+      </c>
+      <c r="J70" s="6">
+        <v>0</v>
+      </c>
+      <c r="L70" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D71" s="5">
+        <v>42186</v>
+      </c>
+      <c r="E71" t="s">
+        <v>1</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G71" s="6">
+        <v>51280</v>
+      </c>
+      <c r="J71" s="6">
+        <v>0</v>
+      </c>
+      <c r="L71" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D72" s="5">
+        <v>42156</v>
+      </c>
+      <c r="E72" t="s">
+        <v>1</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G72" s="6">
+        <v>80762</v>
+      </c>
+      <c r="J72" s="6">
+        <v>0</v>
+      </c>
+      <c r="L72" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D73" s="5">
+        <v>42125</v>
+      </c>
+      <c r="E73" t="s">
+        <v>1</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G73" s="6">
+        <v>76743</v>
+      </c>
+      <c r="J73" s="6">
+        <v>0</v>
+      </c>
+      <c r="L73" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D74" s="5">
+        <v>42095</v>
+      </c>
+      <c r="E74" t="s">
+        <v>1</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G74" s="6">
+        <v>58280</v>
+      </c>
+      <c r="J74" s="6">
+        <v>0</v>
+      </c>
+      <c r="L74" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" t="s">
+        <v>0</v>
+      </c>
+      <c r="C75" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D75" s="5">
+        <v>42064</v>
+      </c>
+      <c r="E75" t="s">
+        <v>1</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G75" s="6">
+        <v>71969</v>
+      </c>
+      <c r="J75" s="6">
+        <v>0</v>
+      </c>
+      <c r="L75" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A76" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D76" s="5">
+        <v>42036</v>
+      </c>
+      <c r="E76" t="s">
+        <v>1</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G76" s="6">
+        <v>57333</v>
+      </c>
+      <c r="J76" s="6">
+        <v>0</v>
+      </c>
+      <c r="L76" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A77" t="s">
+        <v>2</v>
+      </c>
+      <c r="B77" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D77" s="5">
         <v>42005</v>
       </c>
-      <c r="E68" t="s">
-        <v>1</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G68" s="6">
+      <c r="E77" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G77" s="6">
         <v>110615</v>
       </c>
-      <c r="J68" s="6">
-        <v>0</v>
-      </c>
-      <c r="L68" t="s">
+      <c r="J77" s="6">
+        <v>0</v>
+      </c>
+      <c r="L77" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>